<commit_message>
auto:change the form id for labs and medication
</commit_message>
<xml_diff>
--- a/config/forms/app/medication.xlsx
+++ b/config/forms/app/medication.xlsx
@@ -120,7 +120,7 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
-    <t>lmedication</t>
+    <t>medication</t>
   </si>
   <si>
     <t>date</t>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C2" s="18" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-02-10_16-02</v>
+        <v>2023-02-10_16-16</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
auto:adding patient identifier card on the medication form
</commit_message>
<xml_diff>
--- a/config/forms/app/medication.xlsx
+++ b/config/forms/app/medication.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>type</t>
   </si>
@@ -93,6 +93,18 @@
     <t>sex</t>
   </si>
   <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>aka</t>
+  </si>
+  <si>
+    <t>tsis</t>
+  </si>
+  <si>
+    <t>genda</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -120,7 +132,125 @@
     <t>../inputs/contact/name</t>
   </si>
   <si>
+    <t>patient_name1</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name1</t>
+  </si>
+  <si>
+    <t>patient_aka</t>
+  </si>
+  <si>
+    <t>../inputs/contact/aka</t>
+  </si>
+  <si>
+    <t>patient_tsis</t>
+  </si>
+  <si>
+    <t>../inputs/contact/tsis</t>
+  </si>
+  <si>
+    <t>patient_genda</t>
+  </si>
+  <si>
+    <t>../inputs/contact/genda</t>
+  </si>
+  <si>
+    <t>patient_date_of_birth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of birth </t>
+  </si>
+  <si>
+    <t>../inputs/contact/date_of_birth</t>
+  </si>
+  <si>
+    <t>fast_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/fstname != '', instance('contact-summary')/context/fstname, .)</t>
+  </si>
+  <si>
+    <t>last_name_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/lstname != '', instance('contact-summary')/context/lstname, .)</t>
+  </si>
+  <si>
+    <t>date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_date_of_birth != '', instance('contact-summary')/context/patient_date_of_birth, .)</t>
+  </si>
+  <si>
+    <t>aka_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_aka != '', instance('contact-summary')/context/patient_aka, .)</t>
+  </si>
+  <si>
+    <t>tsis_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_tsis != '', instance('contact-summary')/context/patient_tsis, .)</t>
+  </si>
+  <si>
+    <t>at_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_at != '', instance('contact-summary')/context/patient_at, .)</t>
+  </si>
+  <si>
+    <t>yr_date_of_birth_ctx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(int(format-date(today(), "%Y") - format-date(${date_of_birth_ctx}, "%Y")) )
+</t>
+  </si>
+  <si>
+    <t>gender_ctx</t>
+  </si>
+  <si>
+    <t>if(instance('contact-summary')/context/patient_genda != '', instance('contact-summary')/context/patient_genda, .)</t>
+  </si>
+  <si>
     <t>medication</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;i style=”background-color: yellow;”&gt;**${fast_name_ctx}  ${last_name_ctx}**&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 yellow </t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>Nickname: **${aka_ctx}**</t>
+  </si>
+  <si>
+    <t>age_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age: **${yr_date_of_birth_ctx} yr**  </t>
+  </si>
+  <si>
+    <t>gender_n</t>
+  </si>
+  <si>
+    <t>Gender Identity: **${gender_ctx}**</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>TSIS: **${tsis_ctx}**</t>
   </si>
   <si>
     <t>date</t>
@@ -326,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -357,8 +487,17 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -613,7 +752,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="16.25"/>
     <col customWidth="1" min="2" max="2" width="26.0"/>
-    <col customWidth="1" min="3" max="3" width="30.88"/>
+    <col customWidth="1" min="3" max="3" width="46.0"/>
+    <col customWidth="1" min="7" max="7" width="23.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -817,47 +957,85 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="2"/>
@@ -868,32 +1046,68 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -903,10 +1117,14 @@
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -915,26 +1133,38 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -942,71 +1172,49 @@
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>30</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1015,132 +1223,846 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>41</v>
+      <c r="A23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="9"/>
+      <c r="C24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>45</v>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>47</v>
+      <c r="A26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>49</v>
+      <c r="A27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>51</v>
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="12" t="s">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="12" t="s">
-        <v>28</v>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +2082,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1212,26 +2134,26 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>63</v>
+      <c r="A1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1254,25 +2176,25 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="18" t="str">
+      <c r="A2" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="21" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-02-10_16-16</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19" t="s">
-        <v>67</v>
+        <v>2023-07-31_20-31</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>

</xml_diff>